<commit_message>
(C)    Caitlin revisions and corrections
</commit_message>
<xml_diff>
--- a/Suppl/Plan 1.0 - lifting.xlsx
+++ b/Suppl/Plan 1.0 - lifting.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
   <si>
     <t>Day 1</t>
   </si>
@@ -56,18 +56,9 @@
     <t>Style</t>
   </si>
   <si>
-    <t>Super-sets of three -lifts, 1 min break per set</t>
-  </si>
-  <si>
     <t>Get started with trainer's routine</t>
   </si>
   <si>
-    <t>*open pending confirmation</t>
-  </si>
-  <si>
-    <t>(12/7/16) r0</t>
-  </si>
-  <si>
     <t>Shoulders/Triceps ()</t>
   </si>
   <si>
@@ -110,12 +101,6 @@
     <t>Flat Bench Dumbbell Press</t>
   </si>
   <si>
-    <t>Cable Flyes</t>
-  </si>
-  <si>
-    <t>Pec-Dec</t>
-  </si>
-  <si>
     <t>Individual Single Leg Extension</t>
   </si>
   <si>
@@ -128,15 +113,6 @@
     <t>Individual Leg Hamstring Curls</t>
   </si>
   <si>
-    <t>&lt;?&gt; Leg Press</t>
-  </si>
-  <si>
-    <t>&lt;?&gt; Lunges</t>
-  </si>
-  <si>
-    <t>&lt;?&gt; Calf Raise</t>
-  </si>
-  <si>
     <t>Dumbbell Front Raise</t>
   </si>
   <si>
@@ -155,12 +131,6 @@
     <t>Seated Dip Machine</t>
   </si>
   <si>
-    <t>&lt;?&gt; Cable Tricep Extension</t>
-  </si>
-  <si>
-    <t>&lt;?&gt;</t>
-  </si>
-  <si>
     <t>4x15</t>
   </si>
   <si>
@@ -173,9 +143,6 @@
     <t>4x8</t>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;?&gt;</t>
-  </si>
-  <si>
     <t>1 min</t>
   </si>
   <si>
@@ -209,20 +176,50 @@
     <t>4xFail</t>
   </si>
   <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>Init each day with 10 min warm-up walk</t>
-  </si>
-  <si>
     <t>4 Days Lift, 1 Day Cardio, 1 Day Rest</t>
+  </si>
+  <si>
+    <t>Pre</t>
+  </si>
+  <si>
+    <t>Super-sets of two-lifts</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>4x15 ea.</t>
+  </si>
+  <si>
+    <t>Machine Butterfly</t>
+  </si>
+  <si>
+    <t>Cable Crossover Fly</t>
+  </si>
+  <si>
+    <t>Lunges</t>
+  </si>
+  <si>
+    <t>Single Leg No-Weight Calf Raise</t>
+  </si>
+  <si>
+    <t>15 min Elliptical (15/15)</t>
+  </si>
+  <si>
+    <t>10 min warm-up walk</t>
+  </si>
+  <si>
+    <t>(12/7/16) r1</t>
+  </si>
+  <si>
+    <t>Always use weak leg's strength</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +246,12 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -283,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -301,9 +304,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -316,11 +316,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -639,354 +644,352 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K25"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.5703125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.5703125" style="17" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="20">
         <v>42711</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="20"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="1"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="H3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+    </row>
+    <row r="5" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="21"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K5" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="22"/>
+    </row>
+    <row r="6" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="H6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="H6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="E7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="16"/>
+      <c r="E7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="15"/>
       <c r="G7" s="2"/>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J7" s="11"/>
-      <c r="K7" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+        <v>18</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
       <c r="G8" s="2"/>
       <c r="H8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="E9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="16"/>
+      <c r="E9" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="15"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J9" s="11"/>
-      <c r="K9" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="E10" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="16"/>
+      <c r="E10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="15"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="E11" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="16"/>
+      <c r="E11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="15"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="16"/>
+      <c r="E12" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="15"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="13" t="s">
-        <v>23</v>
+      <c r="B13" s="21" t="s">
+        <v>20</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="E13" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="K13" s="16"/>
-    </row>
-    <row r="14" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="E13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="13"/>
       <c r="C14" s="2"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="21"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="19"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="18"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="E16" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="16"/>
+      <c r="E16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="15"/>
       <c r="H16" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" s="15" t="s">
         <v>37</v>
-      </c>
-      <c r="K16" s="16" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="E17" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="16"/>
+      <c r="E17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="15"/>
       <c r="H17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K17" s="16" t="s">
-        <v>60</v>
+      <c r="K17" s="15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="14" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="E18" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="16"/>
+      <c r="E18" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="15"/>
       <c r="H18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="K18" s="16" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="16"/>
+        <v>55</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="15"/>
       <c r="H19" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>45</v>
+        <v>31</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="14" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="E20" s="16">
+      <c r="E20" s="15">
         <v>5</v>
       </c>
-      <c r="F20" s="16"/>
+      <c r="F20" s="15"/>
       <c r="H20" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="K20" s="16" t="s">
-        <v>56</v>
+        <v>32</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -995,84 +998,80 @@
       <c r="C21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="15">
         <v>20</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="15"/>
       <c r="H21" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="K21" s="16" t="s">
-        <v>60</v>
+        <v>33</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="16">
+        <v>42</v>
+      </c>
+      <c r="E22" s="15">
         <v>20</v>
       </c>
-      <c r="F22" s="16"/>
+      <c r="F22" s="15"/>
       <c r="H22" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K22" s="16" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="16"/>
-      <c r="H23" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="K23" s="16" t="s">
-        <v>45</v>
-      </c>
+      <c r="E23" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="H23" s="14"/>
+      <c r="K23" s="15"/>
       <c r="Q23" s="12"/>
       <c r="R23" s="12"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="16">
+        <v>44</v>
+      </c>
+      <c r="E24" s="15">
         <v>40</v>
       </c>
-      <c r="F24" s="16"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="16">
         <v>40</v>
       </c>
-      <c r="F25" s="16"/>
+      <c r="E25" s="15">
+        <v>40</v>
+      </c>
+      <c r="F25" s="15"/>
       <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="2"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J28" s="9" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(C)    meal plan updates
</commit_message>
<xml_diff>
--- a/Suppl/Plan 1.0 - lifting.xlsx
+++ b/Suppl/Plan 1.0 - lifting.xlsx
@@ -9,11 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dec Plan '16 - r0" sheetId="2" r:id="rId1"/>
+    <sheet name="Dec '16 Log" sheetId="3" r:id="rId2"/>
+    <sheet name="Check-in" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Check-in'!$A$1:$D$38</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="120">
   <si>
     <t>Day 1</t>
   </si>
@@ -83,9 +88,6 @@
     <t>*(Wide, Overhand, Narrow)</t>
   </si>
   <si>
-    <t>Individual Dumbbell Preacher Curls</t>
-  </si>
-  <si>
     <t>Individual Incline Dumbbell Curls</t>
   </si>
   <si>
@@ -209,17 +211,195 @@
     <t>10 min warm-up walk</t>
   </si>
   <si>
-    <t>(12/7/16) r1</t>
-  </si>
-  <si>
     <t>Always use weak leg's strength</t>
+  </si>
+  <si>
+    <t>Life Fitness Buddy Names</t>
+  </si>
+  <si>
+    <t>(12/7/16) r2</t>
+  </si>
+  <si>
+    <t>(Lateral Pulldown)</t>
+  </si>
+  <si>
+    <t>(Seated Hammer Strength Rows)</t>
+  </si>
+  <si>
+    <t>(Close Grip Pulldown)</t>
+  </si>
+  <si>
+    <t>(Seated Individual Arm Cable Rows)</t>
+  </si>
+  <si>
+    <t>(Alternating Individual Dumbbell Bicep Curls)</t>
+  </si>
+  <si>
+    <t>(Barbbell Preacher Curls)</t>
+  </si>
+  <si>
+    <t>Barbbell Preacher Curls</t>
+  </si>
+  <si>
+    <t>(Individual Incline Dumbbell Curls)</t>
+  </si>
+  <si>
+    <t>(Dumbbell Bench Press - Incline)</t>
+  </si>
+  <si>
+    <t>(Dumbbell Bench Press - Flat)</t>
+  </si>
+  <si>
+    <t>(Cable Crossover - High)</t>
+  </si>
+  <si>
+    <t>(Selectorized Fly)</t>
+  </si>
+  <si>
+    <t>(Bodyweight Crunch)</t>
+  </si>
+  <si>
+    <t>(Bodyweight Leg Raise)</t>
+  </si>
+  <si>
+    <t>(Bodyweight Plank)</t>
+  </si>
+  <si>
+    <t>(Bodyweight Twist - Russian)</t>
+  </si>
+  <si>
+    <t>(Flutter Kick)</t>
+  </si>
+  <si>
+    <t>(Selectorized Individual Leg Extension)</t>
+  </si>
+  <si>
+    <t>(Dumbbell Step Up - Platform)</t>
+  </si>
+  <si>
+    <t>(Selectorized Leg Curl)</t>
+  </si>
+  <si>
+    <t>(Selectorized Individual Leg Curl)</t>
+  </si>
+  <si>
+    <t>(Bodyweight Lunge)</t>
+  </si>
+  <si>
+    <t>(Stair Bodyweight Calf Raise)</t>
+  </si>
+  <si>
+    <t>(Dumbbell Raise - Front)</t>
+  </si>
+  <si>
+    <t>(Dumbbell Raise - Lateral)</t>
+  </si>
+  <si>
+    <t>(Selectorized Shoulder Press - Overhand)</t>
+  </si>
+  <si>
+    <t>(Cable Face Pull)</t>
+  </si>
+  <si>
+    <t>(Cable Pushdown - Overhand)</t>
+  </si>
+  <si>
+    <t>(Close-Grip Bench Push-Ups)</t>
+  </si>
+  <si>
+    <t>(Seated Dip)</t>
+  </si>
+  <si>
+    <t>finish day 1!</t>
+  </si>
+  <si>
+    <t>draw up all columns</t>
+  </si>
+  <si>
+    <t>(+0)</t>
+  </si>
+  <si>
+    <t>Incline Dumbbell Curls</t>
+  </si>
+  <si>
+    <t>(+5)</t>
+  </si>
+  <si>
+    <t>Single Leg Calf Raise</t>
+  </si>
+  <si>
+    <t>Barbell Preacher Curls</t>
+  </si>
+  <si>
+    <t>(+2)</t>
+  </si>
+  <si>
+    <t>Shoulders/Triceps</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Individual Dumbbell Bicep Curls</t>
+  </si>
+  <si>
+    <t>(+20)</t>
+  </si>
+  <si>
+    <t>(+10)</t>
+  </si>
+  <si>
+    <t>Weighted Step-Ups</t>
+  </si>
+  <si>
+    <t>Single Leg Extension</t>
+  </si>
+  <si>
+    <t>Legs</t>
+  </si>
+  <si>
+    <t>Selectorized Fly</t>
+  </si>
+  <si>
+    <t>Seated Single Arm Cable Rows</t>
+  </si>
+  <si>
+    <t>(-2.5)</t>
+  </si>
+  <si>
+    <t>Incline Bench Dumbbell Press</t>
+  </si>
+  <si>
+    <t>Chest/Abs</t>
+  </si>
+  <si>
+    <t>(+30)</t>
+  </si>
+  <si>
+    <t>Back/Biceps</t>
+  </si>
+  <si>
+    <t>Avg(max reps)</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Avg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d;@"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,16 +436,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -282,11 +508,140 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -319,14 +674,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +1084,7 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -679,10 +1101,10 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="24">
         <v>42711</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -690,35 +1112,35 @@
         <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
+        <v>58</v>
+      </c>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -739,10 +1161,10 @@
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="L5" s="22"/>
+      <c r="K5" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -751,15 +1173,15 @@
       </c>
       <c r="C6" s="2"/>
       <c r="E6" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="15"/>
       <c r="H6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -769,16 +1191,16 @@
       </c>
       <c r="C7" s="2"/>
       <c r="E7" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="2"/>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -791,10 +1213,10 @@
       <c r="F8" s="15"/>
       <c r="G8" s="2"/>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -804,64 +1226,64 @@
       </c>
       <c r="C9" s="2"/>
       <c r="E9" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2"/>
       <c r="E10" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="11"/>
       <c r="K10" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2"/>
       <c r="E11" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2"/>
       <c r="E12" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="2"/>
@@ -869,12 +1291,12 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="21" t="s">
-        <v>20</v>
+      <c r="B13" s="20" t="s">
+        <v>19</v>
       </c>
       <c r="C13" s="2"/>
       <c r="E13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" s="15"/>
       <c r="K13" s="15"/>
@@ -910,75 +1332,75 @@
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2"/>
       <c r="E16" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="15"/>
       <c r="H16" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="2"/>
       <c r="E17" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="15"/>
       <c r="H17" s="14" t="s">
         <v>4</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="2"/>
       <c r="E18" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18" s="15"/>
       <c r="H18" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" s="15"/>
       <c r="H19" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="2"/>
       <c r="E20" s="15">
@@ -986,10 +1408,10 @@
       </c>
       <c r="F20" s="15"/>
       <c r="H20" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -1003,36 +1425,36 @@
       </c>
       <c r="F21" s="15"/>
       <c r="H21" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="15">
         <v>20</v>
       </c>
       <c r="F22" s="15"/>
       <c r="H22" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" s="15" t="s">
         <v>34</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F23" s="15"/>
       <c r="H23" s="14"/>
@@ -1043,7 +1465,7 @@
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E24" s="15">
         <v>40</v>
@@ -1054,7 +1476,7 @@
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E25" s="15">
         <v>40</v>
@@ -1069,9 +1491,258 @@
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J28" s="9" t="s">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="23" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="F39" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="F40" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="F41" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>41</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C47" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B55" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F56" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B61" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J63" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1081,4 +1752,1300 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="25"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="15" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" style="15" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="1.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="1.85546875" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="25"/>
+      <c r="I1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="K1" s="17"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" s="17"/>
+      <c r="Q1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="25"/>
+      <c r="I2" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="28">
+        <v>42711</v>
+      </c>
+      <c r="E3" s="30">
+        <v>60</v>
+      </c>
+      <c r="F3" s="29">
+        <f>(60*15+70*45)/60</f>
+        <v>67.5</v>
+      </c>
+      <c r="H3" s="28">
+        <v>42712</v>
+      </c>
+      <c r="I3" s="30">
+        <v>25</v>
+      </c>
+      <c r="J3" s="39">
+        <f>(25*36 +20*12)/48</f>
+        <v>23.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="28">
+        <v>42717</v>
+      </c>
+      <c r="E4" s="30">
+        <v>70</v>
+      </c>
+      <c r="F4" s="29">
+        <f>(70*45+80*6)/(45+6)</f>
+        <v>71.17647058823529</v>
+      </c>
+      <c r="H4" s="28">
+        <v>42718</v>
+      </c>
+      <c r="I4" s="30">
+        <v>30</v>
+      </c>
+      <c r="J4" s="39">
+        <f>(25*24+30*8+25*10)/(48)</f>
+        <v>22.708333333333332</v>
+      </c>
+      <c r="K4" s="38"/>
+    </row>
+    <row r="5" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="28">
+        <v>42721</v>
+      </c>
+      <c r="E5" s="30">
+        <v>90</v>
+      </c>
+      <c r="F5" s="29">
+        <f>(90*30+80*22)/(52)</f>
+        <v>85.769230769230774</v>
+      </c>
+      <c r="H5" s="28">
+        <v>42722</v>
+      </c>
+      <c r="I5" s="30">
+        <v>30</v>
+      </c>
+      <c r="J5" s="39">
+        <f>(30*26+25*7)/(6+12+8+7)</f>
+        <v>28.939393939393938</v>
+      </c>
+      <c r="K5" s="38"/>
+    </row>
+    <row r="6" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="27">
+        <f>(F5-F3)</f>
+        <v>18.269230769230774</v>
+      </c>
+      <c r="G6" s="30"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="J6" s="32">
+        <f>(J5-J3)</f>
+        <v>5.1893939393939377</v>
+      </c>
+      <c r="K6" s="32"/>
+    </row>
+    <row r="7" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
+      <c r="B7" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="28">
+        <v>42711</v>
+      </c>
+      <c r="E8" s="30">
+        <v>25</v>
+      </c>
+      <c r="F8" s="29">
+        <f>(25*135+27.5*45)/(45*4)</f>
+        <v>25.625</v>
+      </c>
+      <c r="H8" s="28">
+        <v>42712</v>
+      </c>
+      <c r="I8" s="30">
+        <v>30</v>
+      </c>
+      <c r="J8" s="11">
+        <f>(30*10+25*20+20*10)/(40)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
+      <c r="B9" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="28">
+        <v>42717</v>
+      </c>
+      <c r="E9" s="30">
+        <v>35</v>
+      </c>
+      <c r="F9" s="29">
+        <f>(30*45+35*36+30*23+25*45)/(45+36+23+45)</f>
+        <v>29.697986577181208</v>
+      </c>
+      <c r="H9" s="28">
+        <v>42718</v>
+      </c>
+      <c r="I9" s="30">
+        <v>30</v>
+      </c>
+      <c r="J9" s="39">
+        <f>(30*10+30*5+25*14)/(29)</f>
+        <v>27.586206896551722</v>
+      </c>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="28">
+        <v>42721</v>
+      </c>
+      <c r="E10" s="30">
+        <v>35</v>
+      </c>
+      <c r="F10" s="29">
+        <f>(35*45+30*45+30*29)/(45+45+29)</f>
+        <v>31.890756302521009</v>
+      </c>
+      <c r="H10" s="28">
+        <v>42722</v>
+      </c>
+      <c r="I10" s="30">
+        <v>30</v>
+      </c>
+      <c r="J10" s="11">
+        <f>(30*22+35*6+25*6)/(34)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="27">
+        <f>(F10-F8)</f>
+        <v>6.2657563025210088</v>
+      </c>
+      <c r="H11" s="25"/>
+      <c r="I11" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" s="32">
+        <f>(J10-J8)</f>
+        <v>5</v>
+      </c>
+      <c r="K11" s="32"/>
+    </row>
+    <row r="12" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="R12"/>
+    </row>
+    <row r="13" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="28">
+        <v>42711</v>
+      </c>
+      <c r="E13" s="30">
+        <v>70</v>
+      </c>
+      <c r="F13" s="29">
+        <f>(70*24+60*24)/(48)</f>
+        <v>65</v>
+      </c>
+      <c r="H13" s="28">
+        <v>42712</v>
+      </c>
+      <c r="I13" s="30">
+        <v>20</v>
+      </c>
+      <c r="J13" s="37">
+        <f>(20*24+15*26)/(24+26)</f>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="K13" s="30"/>
+    </row>
+    <row r="14" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
+      <c r="B14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="28">
+        <v>42717</v>
+      </c>
+      <c r="E14" s="30">
+        <v>80</v>
+      </c>
+      <c r="F14" s="29">
+        <f>(80*15+70*39)/(15+39)</f>
+        <v>72.777777777777771</v>
+      </c>
+      <c r="H14" s="28">
+        <v>42718</v>
+      </c>
+      <c r="I14" s="30">
+        <v>17.5</v>
+      </c>
+      <c r="J14" s="36">
+        <f>(15*24+17.5*25)/(24+25)</f>
+        <v>16.275510204081634</v>
+      </c>
+      <c r="K14" s="30"/>
+    </row>
+    <row r="15" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="28">
+        <v>42721</v>
+      </c>
+      <c r="E15" s="30">
+        <v>90</v>
+      </c>
+      <c r="F15" s="29">
+        <f>(90*24+80*24)/(48)</f>
+        <v>85</v>
+      </c>
+      <c r="H15" s="28">
+        <v>42722</v>
+      </c>
+      <c r="I15" s="30">
+        <v>17.5</v>
+      </c>
+      <c r="J15" s="36">
+        <f>(17.5*24+15*24)/(24+24)</f>
+        <v>16.25</v>
+      </c>
+      <c r="K15" s="30"/>
+    </row>
+    <row r="16" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" s="27">
+        <f>(F15-F13)</f>
+        <v>20</v>
+      </c>
+      <c r="G16" s="30"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="J16" s="35">
+        <f>(J15-J13)</f>
+        <v>-1.1499999999999986</v>
+      </c>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+    </row>
+    <row r="17" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q17" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="28">
+        <v>42711</v>
+      </c>
+      <c r="E18" s="15">
+        <v>30</v>
+      </c>
+      <c r="F18" s="29">
+        <f>(30*30+40*2)/(32)</f>
+        <v>30.625</v>
+      </c>
+      <c r="G18"/>
+      <c r="H18" s="28">
+        <v>42712</v>
+      </c>
+      <c r="I18" s="15">
+        <v>50</v>
+      </c>
+      <c r="J18" s="9">
+        <v>50</v>
+      </c>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="28">
+        <v>42717</v>
+      </c>
+      <c r="E19" s="30">
+        <v>30</v>
+      </c>
+      <c r="F19" s="29">
+        <f>(30*32+20*15)/(32+15)</f>
+        <v>26.808510638297872</v>
+      </c>
+      <c r="H19" s="28">
+        <v>42718</v>
+      </c>
+      <c r="I19" s="30">
+        <v>70</v>
+      </c>
+      <c r="J19" s="34">
+        <f>(60*36+70*8)/(36+8)</f>
+        <v>61.81818181818182</v>
+      </c>
+      <c r="K19" s="30"/>
+    </row>
+    <row r="20" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="28">
+        <v>42721</v>
+      </c>
+      <c r="E20" s="30">
+        <v>40</v>
+      </c>
+      <c r="F20" s="29">
+        <f>(40*4+30*30)/(34)</f>
+        <v>31.176470588235293</v>
+      </c>
+      <c r="H20" s="28">
+        <v>42722</v>
+      </c>
+      <c r="I20" s="30">
+        <v>70</v>
+      </c>
+      <c r="J20" s="33">
+        <f>(70*39)/(39)</f>
+        <v>70</v>
+      </c>
+      <c r="K20" s="30"/>
+    </row>
+    <row r="21" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
+      <c r="B21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="28"/>
+      <c r="E21" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" s="27">
+        <f>(F20-F18)</f>
+        <v>0.55147058823529349</v>
+      </c>
+      <c r="H21" s="28"/>
+      <c r="I21" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="J21" s="32">
+        <f>(J20-J18)</f>
+        <v>20</v>
+      </c>
+      <c r="K21" s="30"/>
+    </row>
+    <row r="22" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="23"/>
+      <c r="B22" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="28"/>
+      <c r="E22" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q22" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="23"/>
+      <c r="B23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="28">
+        <v>42711</v>
+      </c>
+      <c r="E23" s="30">
+        <v>15</v>
+      </c>
+      <c r="F23" s="29">
+        <f>(15*17)/(17)</f>
+        <v>15</v>
+      </c>
+      <c r="H23" s="28">
+        <v>42712</v>
+      </c>
+      <c r="I23" s="30">
+        <v>1</v>
+      </c>
+      <c r="J23" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="K23" s="30"/>
+    </row>
+    <row r="24" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
+      <c r="B24" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="28">
+        <v>42717</v>
+      </c>
+      <c r="E24" s="30">
+        <v>20</v>
+      </c>
+      <c r="F24" s="29">
+        <f>(20*9+15*23)/(9+23)</f>
+        <v>16.40625</v>
+      </c>
+      <c r="H24" s="28">
+        <v>42718</v>
+      </c>
+      <c r="I24" s="30">
+        <v>2</v>
+      </c>
+      <c r="J24" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="K24" s="30"/>
+    </row>
+    <row r="25" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="23"/>
+      <c r="D25" s="28">
+        <v>42721</v>
+      </c>
+      <c r="E25" s="30">
+        <v>20</v>
+      </c>
+      <c r="F25" s="29">
+        <f>(20*15+15*9)/(15+9)</f>
+        <v>18.125</v>
+      </c>
+      <c r="H25" s="28">
+        <v>42722</v>
+      </c>
+      <c r="I25" s="30">
+        <v>3</v>
+      </c>
+      <c r="J25" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="K25" s="30"/>
+    </row>
+    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="27">
+        <f>(F25-F23)</f>
+        <v>3.125</v>
+      </c>
+      <c r="H26" s="25"/>
+      <c r="I26" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="J26" s="30"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+    </row>
+    <row r="27" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="28"/>
+      <c r="E27" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="28"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q27" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="28">
+        <v>42711</v>
+      </c>
+      <c r="E28" s="15">
+        <v>15</v>
+      </c>
+      <c r="F28" s="29">
+        <f>(10*12+15*12)/(24)</f>
+        <v>12.5</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+    </row>
+    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="28">
+        <v>42717</v>
+      </c>
+      <c r="E29" s="15">
+        <v>15</v>
+      </c>
+      <c r="F29" s="29">
+        <f>(10*22+15*4)/(26)</f>
+        <v>10.76923076923077</v>
+      </c>
+      <c r="G29"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+    </row>
+    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="28">
+        <v>42721</v>
+      </c>
+      <c r="E30" s="15">
+        <v>20</v>
+      </c>
+      <c r="F30" s="29">
+        <f>(10*36+20*6)/(36+6)</f>
+        <v>11.428571428571429</v>
+      </c>
+      <c r="H30" s="28"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+    </row>
+    <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F31" s="27">
+        <f>(F30-F28)</f>
+        <v>-1.0714285714285712</v>
+      </c>
+      <c r="H31" s="25"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+    </row>
+    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H32" s="25"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+    </row>
+    <row r="33" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="28">
+        <v>42711</v>
+      </c>
+      <c r="E33" s="15">
+        <v>15</v>
+      </c>
+      <c r="F33" s="29">
+        <f>(15*15)/(15)</f>
+        <v>15</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="Q33" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="28">
+        <v>42717</v>
+      </c>
+      <c r="E34" s="15">
+        <v>15</v>
+      </c>
+      <c r="F34" s="29">
+        <f>(15*11+10*8)/(11+8)</f>
+        <v>12.894736842105264</v>
+      </c>
+      <c r="G34"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+    </row>
+    <row r="35" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="28">
+        <v>42721</v>
+      </c>
+      <c r="E35" s="15">
+        <v>15</v>
+      </c>
+      <c r="F35" s="29">
+        <f>(15*12+10*24)/(36)</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="G35"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+    </row>
+    <row r="36" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="11"/>
+      <c r="E36" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" s="27">
+        <f>(F35-F33)</f>
+        <v>-3.3333333333333339</v>
+      </c>
+      <c r="H36" s="25"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B39" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="52" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25"/>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="15"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="48">
+        <v>42711</v>
+      </c>
+      <c r="B4" s="51">
+        <v>60</v>
+      </c>
+      <c r="C4" s="46">
+        <f>(60*15+70*45)/60</f>
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="45">
+        <v>42717</v>
+      </c>
+      <c r="B5" s="50">
+        <v>70</v>
+      </c>
+      <c r="C5" s="43">
+        <f>(70*45+80*6)/(45+6)</f>
+        <v>71.17647058823529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="42">
+        <v>42721</v>
+      </c>
+      <c r="B6" s="49">
+        <v>90</v>
+      </c>
+      <c r="C6" s="40">
+        <f>(90*30+80*22)/(52)</f>
+        <v>85.769230769230774</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="27">
+        <f>(C6-C4)</f>
+        <v>18.269230769230774</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="28"/>
+      <c r="B8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="30"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="48">
+        <v>42711</v>
+      </c>
+      <c r="B9" s="51">
+        <v>25</v>
+      </c>
+      <c r="C9" s="46">
+        <f>(25*135+27.5*45)/(45*4)</f>
+        <v>25.625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="45">
+        <v>42717</v>
+      </c>
+      <c r="B10" s="50">
+        <v>35</v>
+      </c>
+      <c r="C10" s="43">
+        <f>(30*45+35*36+30*23+25*45)/(45+36+23+45)</f>
+        <v>29.697986577181208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="42">
+        <v>42721</v>
+      </c>
+      <c r="B11" s="49">
+        <v>35</v>
+      </c>
+      <c r="C11" s="40">
+        <f>(35*45+30*45+30*29)/(45+45+29)</f>
+        <v>31.890756302521009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="27">
+        <f>(C11-C9)</f>
+        <v>6.2657563025210088</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="28"/>
+      <c r="B13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="30"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="48">
+        <v>42711</v>
+      </c>
+      <c r="B14" s="51">
+        <v>70</v>
+      </c>
+      <c r="C14" s="46">
+        <f>(70*24+60*24)/(48)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="45">
+        <v>42717</v>
+      </c>
+      <c r="B15" s="50">
+        <v>80</v>
+      </c>
+      <c r="C15" s="43">
+        <f>(80*15+70*39)/(15+39)</f>
+        <v>72.777777777777771</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="42">
+        <v>42721</v>
+      </c>
+      <c r="B16" s="49">
+        <v>90</v>
+      </c>
+      <c r="C16" s="40">
+        <f>(90*24+80*24)/(48)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="27">
+        <f>(C16-C14)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28"/>
+      <c r="B18" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="30"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="48">
+        <v>42711</v>
+      </c>
+      <c r="B19" s="47">
+        <v>30</v>
+      </c>
+      <c r="C19" s="46">
+        <f>(30*30+40*2)/(32)</f>
+        <v>30.625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="45">
+        <v>42717</v>
+      </c>
+      <c r="B20" s="50">
+        <v>30</v>
+      </c>
+      <c r="C20" s="43">
+        <f>(30*32+20*15)/(32+15)</f>
+        <v>26.808510638297872</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="42">
+        <v>42721</v>
+      </c>
+      <c r="B21" s="49">
+        <v>40</v>
+      </c>
+      <c r="C21" s="40">
+        <f>(40*4+30*30)/(34)</f>
+        <v>31.176470588235293</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="27">
+        <f>(C21-C19)</f>
+        <v>0.55147058823529349</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="28"/>
+      <c r="B23" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="30"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="48">
+        <v>42711</v>
+      </c>
+      <c r="B24" s="51">
+        <v>15</v>
+      </c>
+      <c r="C24" s="46">
+        <f>(15*17)/(17)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="45">
+        <v>42717</v>
+      </c>
+      <c r="B25" s="50">
+        <v>20</v>
+      </c>
+      <c r="C25" s="43">
+        <f>(20*9+15*23)/(9+23)</f>
+        <v>16.40625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="42">
+        <v>42721</v>
+      </c>
+      <c r="B26" s="49">
+        <v>20</v>
+      </c>
+      <c r="C26" s="40">
+        <f>(20*15+15*9)/(15+9)</f>
+        <v>18.125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="27">
+        <f>(C26-C24)</f>
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="28"/>
+      <c r="B28" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="30"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="48">
+        <v>42711</v>
+      </c>
+      <c r="B29" s="47">
+        <v>15</v>
+      </c>
+      <c r="C29" s="46">
+        <f>(10*12+15*12)/(24)</f>
+        <v>12.5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="45">
+        <v>42717</v>
+      </c>
+      <c r="B30" s="44">
+        <v>15</v>
+      </c>
+      <c r="C30" s="43">
+        <f>(10*22+15*4)/(26)</f>
+        <v>10.76923076923077</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="42">
+        <v>42721</v>
+      </c>
+      <c r="B31" s="41">
+        <v>20</v>
+      </c>
+      <c r="C31" s="40">
+        <f>(10*36+20*6)/(36+6)</f>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
+      <c r="B32" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="27">
+        <f>(C31-C29)</f>
+        <v>-1.0714285714285712</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="25"/>
+      <c r="B33" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="15"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="48">
+        <v>42711</v>
+      </c>
+      <c r="B34" s="47">
+        <v>15</v>
+      </c>
+      <c r="C34" s="46">
+        <f>(15*15)/(15)</f>
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="45">
+        <v>42717</v>
+      </c>
+      <c r="B35" s="44">
+        <v>15</v>
+      </c>
+      <c r="C35" s="43">
+        <f>(15*11+10*8)/(11+8)</f>
+        <v>12.894736842105264</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="42">
+        <v>42721</v>
+      </c>
+      <c r="B36" s="41">
+        <v>15</v>
+      </c>
+      <c r="C36" s="40">
+        <f>(15*12+10*24)/(36)</f>
+        <v>11.666666666666666</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="27">
+        <f>(C36-C34)</f>
+        <v>-3.3333333333333339</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="25"/>
+      <c r="C38" s="15"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="25"/>
+      <c r="C39" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
(C)    updates to diet (1700 cal) and workout routine (matches        current activities
</commit_message>
<xml_diff>
--- a/Suppl/Plan 1.0 - lifting.xlsx
+++ b/Suppl/Plan 1.0 - lifting.xlsx
@@ -9,15 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Dec Plan '16 - r0" sheetId="2" r:id="rId1"/>
     <sheet name="Dec '16 Log" sheetId="3" r:id="rId2"/>
-    <sheet name="Check-in" sheetId="4" r:id="rId3"/>
+    <sheet name="BB Check" sheetId="4" r:id="rId3"/>
+    <sheet name="Legs Check" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Check-in'!$A$1:$D$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'BB Check'!$A$1:$D$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Legs Check'!$A$1:$D$24</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="128">
   <si>
     <t>Day 1</t>
   </si>
@@ -389,6 +391,30 @@
   </si>
   <si>
     <t>Avg</t>
+  </si>
+  <si>
+    <t>12/9</t>
+  </si>
+  <si>
+    <t>12/15</t>
+  </si>
+  <si>
+    <t>12/19</t>
+  </si>
+  <si>
+    <t>()</t>
+  </si>
+  <si>
+    <t>(12/24/16)</t>
+  </si>
+  <si>
+    <t>(+25)</t>
+  </si>
+  <si>
+    <t>(+40)</t>
+  </si>
+  <si>
+    <t>(12/26/16)</t>
   </si>
 </sst>
 </file>
@@ -399,7 +425,7 @@
     <numFmt numFmtId="164" formatCode="m/d;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,6 +498,14 @@
       <b/>
       <sz val="26"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -641,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -680,9 +714,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -749,6 +780,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1101,10 +1153,10 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="59">
         <v>42711</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="59"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -1758,23 +1810,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F38"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="W40" sqref="W40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="25"/>
+    <col min="4" max="4" width="9.140625" style="24"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" style="15" customWidth="1"/>
     <col min="7" max="7" width="1.85546875" style="15" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="1.85546875" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="52"/>
     <col min="14" max="14" width="13.5703125" customWidth="1"/>
     <col min="15" max="15" width="1.85546875" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="15"/>
+    <col min="18" max="18" width="13.7109375" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -1784,7 +1838,7 @@
       <c r="F1" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="25"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="15" t="s">
         <v>117</v>
       </c>
@@ -1792,7 +1846,6 @@
         <v>116</v>
       </c>
       <c r="K1" s="17"/>
-      <c r="L1" s="15"/>
       <c r="M1" s="15" t="s">
         <v>117</v>
       </c>
@@ -1803,28 +1856,27 @@
       <c r="Q1" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="R1" s="15" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>115</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="25"/>
+      <c r="H2" s="24"/>
       <c r="I2" s="11" t="s">
         <v>112</v>
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
       <c r="M2" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="29" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1833,25 +1885,45 @@
       <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="27">
         <v>42711</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="29">
         <v>60</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="28">
         <f>(60*15+70*45)/60</f>
         <v>67.5</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="27">
         <v>42712</v>
       </c>
-      <c r="I3" s="30">
+      <c r="I3" s="29">
         <v>25</v>
       </c>
-      <c r="J3" s="39">
+      <c r="J3" s="38">
         <f>(25*36 +20*12)/48</f>
         <v>23.75</v>
+      </c>
+      <c r="L3" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="M3" s="29">
+        <v>40</v>
+      </c>
+      <c r="N3" s="29">
+        <f>(40*12+30*12+35*12)/(12+12+12)</f>
+        <v>35</v>
+      </c>
+      <c r="P3" s="60">
+        <v>42716</v>
+      </c>
+      <c r="Q3" s="29">
+        <v>10</v>
+      </c>
+      <c r="R3" s="54">
+        <f>(10*27+5*10)/(37)</f>
+        <v>8.6486486486486491</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1859,128 +1931,203 @@
       <c r="B4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="27">
         <v>42717</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="29">
         <v>70</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="28">
         <f>(70*45+80*6)/(45+6)</f>
         <v>71.17647058823529</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="27">
         <v>42718</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="29">
         <v>30</v>
       </c>
-      <c r="J4" s="39">
+      <c r="J4" s="38">
         <f>(25*24+30*8+25*10)/(48)</f>
         <v>22.708333333333332</v>
       </c>
-      <c r="K4" s="38"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="M4" s="29">
+        <v>40</v>
+      </c>
+      <c r="N4" s="54">
+        <f>(40*12+35*36)/(48)</f>
+        <v>36.25</v>
+      </c>
+      <c r="P4" s="60">
+        <v>42720</v>
+      </c>
+      <c r="Q4" s="29">
+        <v>15</v>
+      </c>
+      <c r="R4" s="54">
+        <f>(15*10+10*10+5*10)/(30)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="27">
         <v>42721</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <v>90</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="28">
         <f>(90*30+80*22)/(52)</f>
         <v>85.769230769230774</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="27">
         <v>42722</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="29">
         <v>30</v>
       </c>
-      <c r="J5" s="39">
+      <c r="J5" s="38">
         <f>(30*26+25*7)/(6+12+8+7)</f>
         <v>28.939393939393938</v>
       </c>
-      <c r="K5" s="38"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="M5" s="29">
+        <v>50</v>
+      </c>
+      <c r="N5" s="54">
+        <f>(50*8+40*12+35*12)/(8+12+12)</f>
+        <v>40.625</v>
+      </c>
+      <c r="P5" s="60">
+        <v>42725</v>
+      </c>
+      <c r="Q5" s="29">
+        <v>15</v>
+      </c>
+      <c r="R5" s="54">
+        <f>(15*19+10*10)/(29)</f>
+        <v>13.275862068965518</v>
+      </c>
     </row>
     <row r="6" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="B6" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="26" t="s">
+      <c r="D6" s="27"/>
+      <c r="E6" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="26">
         <f>(F5-F3)</f>
         <v>18.269230769230774</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="26" t="s">
+      <c r="G6" s="29"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="31">
         <f>(J5-J3)</f>
         <v>5.1893939393939377</v>
       </c>
-      <c r="K6" s="32"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="N6" s="26">
+        <f>(N5-N3)</f>
+        <v>5.625</v>
+      </c>
+      <c r="Q6" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="R6" s="26">
+        <f>(R5-R3)</f>
+        <v>4.6272134203168687</v>
+      </c>
     </row>
     <row r="7" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
       <c r="B7" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="28"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="27"/>
       <c r="I7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="53"/>
       <c r="M7" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="Q7" s="11" t="s">
+      <c r="Q7" s="29" t="s">
         <v>4</v>
       </c>
+      <c r="R7" s="29"/>
     </row>
     <row r="8" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
       <c r="B8" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="27">
         <v>42711</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="29">
         <v>25</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="28">
         <f>(25*135+27.5*45)/(45*4)</f>
         <v>25.625</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="27">
         <v>42712</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="29">
         <v>30</v>
       </c>
       <c r="J8" s="11">
         <f>(30*10+25*20+20*10)/(40)</f>
         <v>25</v>
+      </c>
+      <c r="L8" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="M8" s="29">
+        <v>25</v>
+      </c>
+      <c r="N8" s="54">
+        <f>(20*10+25*20)/(30)</f>
+        <v>23.333333333333332</v>
+      </c>
+      <c r="P8" s="60">
+        <v>42716</v>
+      </c>
+      <c r="Q8" s="29">
+        <v>5</v>
+      </c>
+      <c r="R8" s="54">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1988,241 +2135,371 @@
       <c r="B9" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="27">
         <v>42717</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <v>35</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="28">
         <f>(30*45+35*36+30*23+25*45)/(45+36+23+45)</f>
         <v>29.697986577181208</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="27">
         <v>42718</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="29">
         <v>30</v>
       </c>
-      <c r="J9" s="39">
+      <c r="J9" s="38">
         <f>(30*10+30*5+25*14)/(29)</f>
         <v>27.586206896551722</v>
       </c>
-      <c r="K9" s="38"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="M9" s="29">
+        <v>30</v>
+      </c>
+      <c r="N9" s="54">
+        <f>(25*30+30*10)/(40)</f>
+        <v>26.25</v>
+      </c>
+      <c r="P9" s="60">
+        <v>42720</v>
+      </c>
+      <c r="Q9" s="29">
+        <v>10</v>
+      </c>
+      <c r="R9" s="54">
+        <f>(5*40+10*20)/(60)</f>
+        <v>6.666666666666667</v>
+      </c>
     </row>
     <row r="10" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="28">
+      <c r="D10" s="27">
         <v>42721</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="29">
         <v>35</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="28">
         <f>(35*45+30*45+30*29)/(45+45+29)</f>
         <v>31.890756302521009</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="27">
         <v>42722</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="29">
         <v>30</v>
       </c>
       <c r="J10" s="11">
         <f>(30*22+35*6+25*6)/(34)</f>
         <v>30</v>
       </c>
+      <c r="L10" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="M10" s="29">
+        <v>30</v>
+      </c>
+      <c r="N10" s="29">
+        <f>(30*38)/(38)</f>
+        <v>30</v>
+      </c>
+      <c r="P10" s="60">
+        <v>42725</v>
+      </c>
+      <c r="Q10" s="29">
+        <v>10</v>
+      </c>
+      <c r="R10" s="54">
+        <f>(10*21+5*40)/(61)</f>
+        <v>6.721311475409836</v>
+      </c>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="26">
         <f>(F10-F8)</f>
         <v>6.2657563025210088</v>
       </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="26" t="s">
+      <c r="H11" s="24"/>
+      <c r="I11" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="J11" s="32">
+      <c r="J11" s="31">
         <f>(J10-J8)</f>
         <v>5</v>
       </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="N11" s="26">
+        <f>(N10-N8)</f>
+        <v>6.6666666666666679</v>
+      </c>
+      <c r="Q11" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="R11" s="26">
+        <f>(R10-R8)</f>
+        <v>1.721311475409836</v>
+      </c>
     </row>
     <row r="12" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="28"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="27"/>
       <c r="I12" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="53"/>
       <c r="M12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="Q12" s="11" t="s">
+      <c r="Q12" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="R12"/>
+      <c r="R12" s="15"/>
     </row>
     <row r="13" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
       <c r="B13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="27">
         <v>42711</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="29">
         <v>70</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="28">
         <f>(70*24+60*24)/(48)</f>
         <v>65</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="27">
         <v>42712</v>
       </c>
-      <c r="I13" s="30">
+      <c r="I13" s="29">
         <v>20</v>
       </c>
-      <c r="J13" s="37">
+      <c r="J13" s="36">
         <f>(20*24+15*26)/(24+26)</f>
         <v>17.399999999999999</v>
       </c>
-      <c r="K13" s="30"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="M13" s="29">
+        <v>65</v>
+      </c>
+      <c r="N13" s="54">
+        <f>(50*30+60*6)/(36)</f>
+        <v>51.666666666666664</v>
+      </c>
+      <c r="P13" s="60">
+        <v>42716</v>
+      </c>
+      <c r="Q13" s="29">
+        <v>50</v>
+      </c>
+      <c r="R13" s="54">
+        <f>(50*5+40*30)/(35)</f>
+        <v>41.428571428571431</v>
+      </c>
     </row>
     <row r="14" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
       <c r="B14" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="27">
         <v>42717</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="29">
         <v>80</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="28">
         <f>(80*15+70*39)/(15+39)</f>
         <v>72.777777777777771</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="27">
         <v>42718</v>
       </c>
-      <c r="I14" s="30">
+      <c r="I14" s="29">
         <v>17.5</v>
       </c>
-      <c r="J14" s="36">
+      <c r="J14" s="35">
         <f>(15*24+17.5*25)/(24+25)</f>
         <v>16.275510204081634</v>
       </c>
-      <c r="K14" s="30"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="M14" s="29">
+        <v>60</v>
+      </c>
+      <c r="N14" s="54">
+        <f>(50*15+55*30+60*10)/(15+30+10)</f>
+        <v>54.545454545454547</v>
+      </c>
+      <c r="P14" s="60">
+        <v>42720</v>
+      </c>
+      <c r="Q14" s="29">
+        <v>50</v>
+      </c>
+      <c r="R14" s="54">
+        <f>(50*18+40*10+45*7)/(18+7+10)</f>
+        <v>46.142857142857146</v>
+      </c>
     </row>
     <row r="15" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
       <c r="B15" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="27">
         <v>42721</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="29">
         <v>90</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="28">
         <f>(90*24+80*24)/(48)</f>
         <v>85</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="27">
         <v>42722</v>
       </c>
-      <c r="I15" s="30">
+      <c r="I15" s="29">
         <v>17.5</v>
       </c>
-      <c r="J15" s="36">
+      <c r="J15" s="35">
         <f>(17.5*24+15*24)/(24+24)</f>
         <v>16.25</v>
       </c>
-      <c r="K15" s="30"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="M15" s="29">
+        <v>70</v>
+      </c>
+      <c r="N15" s="54">
+        <f>(70*9+60*40)/(49)</f>
+        <v>61.836734693877553</v>
+      </c>
+      <c r="P15" s="60">
+        <v>42725</v>
+      </c>
+      <c r="Q15" s="29">
+        <v>60</v>
+      </c>
+      <c r="R15" s="29">
+        <f>(60*10+55*16+50*10)/(10+16+10)</f>
+        <v>55</v>
+      </c>
     </row>
     <row r="16" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
       <c r="B16" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="26" t="s">
+      <c r="D16" s="27"/>
+      <c r="E16" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="26">
         <f>(F15-F13)</f>
         <v>20</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="26" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="J16" s="35">
+      <c r="J16" s="34">
         <f>(J15-J13)</f>
         <v>-1.1499999999999986</v>
       </c>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-    </row>
-    <row r="17" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="29"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="N16" s="26">
+        <f>(N15-N13)</f>
+        <v>10.170068027210888</v>
+      </c>
+      <c r="Q16" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="R16" s="26">
+        <f>(R15-R13)</f>
+        <v>13.571428571428569</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
-      <c r="D17" s="28"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="27"/>
       <c r="I17" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="53"/>
       <c r="M17" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="Q17" s="11" t="s">
+      <c r="Q17" s="29" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="31" t="s">
+      <c r="R17" s="29"/>
+    </row>
+    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="27">
         <v>42711</v>
       </c>
       <c r="E18" s="15">
         <v>30</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="28">
         <f>(30*30+40*2)/(32)</f>
         <v>30.625</v>
       </c>
       <c r="G18"/>
-      <c r="H18" s="28">
+      <c r="H18" s="27">
         <v>42712</v>
       </c>
       <c r="I18" s="15">
@@ -2232,385 +2509,558 @@
         <v>50</v>
       </c>
       <c r="K18" s="15"/>
-    </row>
-    <row r="19" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L18" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="M18" s="29">
+        <v>35</v>
+      </c>
+      <c r="N18" s="55">
+        <f>(30*8+35*16)/(24)</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="P18" s="60">
+        <v>42716</v>
+      </c>
+      <c r="Q18" s="29">
+        <v>60</v>
+      </c>
+      <c r="R18" s="15">
+        <f>(60*45)/(45)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23"/>
       <c r="B19" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="28">
+      <c r="D19" s="27">
         <v>42717</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="29">
         <v>30</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="28">
         <f>(30*32+20*15)/(32+15)</f>
         <v>26.808510638297872</v>
       </c>
-      <c r="H19" s="28">
+      <c r="H19" s="27">
         <v>42718</v>
       </c>
-      <c r="I19" s="30">
+      <c r="I19" s="29">
         <v>70</v>
       </c>
-      <c r="J19" s="34">
+      <c r="J19" s="33">
         <f>(60*36+70*8)/(36+8)</f>
         <v>61.81818181818182</v>
       </c>
-      <c r="K19" s="30"/>
-    </row>
-    <row r="20" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="29"/>
+      <c r="L19" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="M19" s="29">
+        <v>35</v>
+      </c>
+      <c r="N19" s="54">
+        <f>(30*15+35*24)/(39)</f>
+        <v>33.07692307692308</v>
+      </c>
+      <c r="P19" s="60">
+        <v>42720</v>
+      </c>
+      <c r="Q19" s="29">
+        <v>80</v>
+      </c>
+      <c r="R19" s="54">
+        <f>(60*30+70*15+80*15)/(60)</f>
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
       <c r="B20" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="28">
+      <c r="D20" s="27">
         <v>42721</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="29">
         <v>40</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="28">
         <f>(40*4+30*30)/(34)</f>
         <v>31.176470588235293</v>
       </c>
-      <c r="H20" s="28">
+      <c r="H20" s="27">
         <v>42722</v>
       </c>
-      <c r="I20" s="30">
+      <c r="I20" s="29">
         <v>70</v>
       </c>
-      <c r="J20" s="33">
+      <c r="J20" s="32">
         <f>(70*39)/(39)</f>
         <v>70</v>
       </c>
-      <c r="K20" s="30"/>
-    </row>
-    <row r="21" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="29"/>
+      <c r="L20" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="M20" s="29">
+        <v>40</v>
+      </c>
+      <c r="N20" s="54">
+        <f>(35*24+40*6)/(30)</f>
+        <v>36</v>
+      </c>
+      <c r="P20" s="60">
+        <v>42725</v>
+      </c>
+      <c r="Q20" s="29">
+        <v>80</v>
+      </c>
+      <c r="R20" s="54">
+        <f>(80*23+60*15)/(23+15)</f>
+        <v>72.10526315789474</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
       <c r="B21" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="26" t="s">
+      <c r="D21" s="27"/>
+      <c r="E21" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F21" s="26">
         <f>(F20-F18)</f>
         <v>0.55147058823529349</v>
       </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="26" t="s">
+      <c r="H21" s="27"/>
+      <c r="I21" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="J21" s="32">
+      <c r="J21" s="31">
         <f>(J20-J18)</f>
         <v>20</v>
       </c>
-      <c r="K21" s="30"/>
-    </row>
-    <row r="22" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="29"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="N21" s="26">
+        <f>(N20-N18)</f>
+        <v>2.6666666666666643</v>
+      </c>
+      <c r="Q21" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="R21" s="26">
+        <f>(R20-R18)</f>
+        <v>12.10526315789474</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="28"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="28"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="27"/>
       <c r="I22" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="53"/>
       <c r="M22" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="Q22" s="11" t="s">
+      <c r="Q22" s="29" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R22" s="29"/>
+    </row>
+    <row r="23" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
       <c r="B23" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="28">
+      <c r="D23" s="27">
         <v>42711</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="29">
         <v>15</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="28">
         <f>(15*17)/(17)</f>
         <v>15</v>
       </c>
-      <c r="H23" s="28">
+      <c r="H23" s="27">
         <v>42712</v>
       </c>
-      <c r="I23" s="30">
+      <c r="I23" s="29">
         <v>1</v>
       </c>
-      <c r="J23" s="30" t="s">
+      <c r="J23" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="K23" s="30"/>
-    </row>
-    <row r="24" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="29"/>
+      <c r="L23" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="M23" s="29">
+        <v>16</v>
+      </c>
+      <c r="N23" s="29">
+        <v>16</v>
+      </c>
+      <c r="P23" s="60">
+        <v>42716</v>
+      </c>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+    </row>
+    <row r="24" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="28">
+      <c r="D24" s="27">
         <v>42717</v>
       </c>
-      <c r="E24" s="30">
+      <c r="E24" s="29">
         <v>20</v>
       </c>
-      <c r="F24" s="29">
+      <c r="F24" s="28">
         <f>(20*9+15*23)/(9+23)</f>
         <v>16.40625</v>
       </c>
-      <c r="H24" s="28">
+      <c r="H24" s="27">
         <v>42718</v>
       </c>
-      <c r="I24" s="30">
+      <c r="I24" s="29">
         <v>2</v>
       </c>
-      <c r="J24" s="30" t="s">
+      <c r="J24" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="K24" s="30"/>
-    </row>
-    <row r="25" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K24" s="29"/>
+      <c r="L24" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="M24" s="29">
+        <v>16</v>
+      </c>
+      <c r="N24" s="29">
+        <v>16</v>
+      </c>
+      <c r="P24" s="60">
+        <v>42720</v>
+      </c>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+    </row>
+    <row r="25" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
-      <c r="D25" s="28">
+      <c r="D25" s="27">
         <v>42721</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="29">
         <v>20</v>
       </c>
-      <c r="F25" s="29">
+      <c r="F25" s="28">
         <f>(20*15+15*9)/(15+9)</f>
         <v>18.125</v>
       </c>
-      <c r="H25" s="28">
+      <c r="H25" s="27">
         <v>42722</v>
       </c>
-      <c r="I25" s="30">
+      <c r="I25" s="29">
         <v>3</v>
       </c>
-      <c r="J25" s="30" t="s">
+      <c r="J25" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="K25" s="30"/>
-    </row>
-    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="31" t="s">
+      <c r="K25" s="29"/>
+      <c r="L25" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="M25" s="29">
+        <v>16</v>
+      </c>
+      <c r="N25" s="29">
+        <v>16</v>
+      </c>
+      <c r="P25" s="60">
+        <v>42725</v>
+      </c>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="29"/>
+    </row>
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="26">
         <f>(F25-F23)</f>
         <v>3.125</v>
       </c>
-      <c r="H26" s="25"/>
-      <c r="I26" s="26" t="s">
+      <c r="H26" s="24"/>
+      <c r="I26" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="J26" s="30"/>
+      <c r="J26" s="29"/>
       <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-    </row>
-    <row r="27" spans="1:17" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L26" s="53"/>
+      <c r="M26" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="N26" s="56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="28"/>
+      <c r="D27" s="27"/>
       <c r="E27" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="28"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="27"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="53"/>
       <c r="M27" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="Q27" s="11" t="s">
+      <c r="Q27" s="29" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R27" s="29"/>
+    </row>
+    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="28">
+      <c r="D28" s="27">
         <v>42711</v>
       </c>
       <c r="E28" s="15">
         <v>15</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="28">
         <f>(10*12+15*12)/(24)</f>
         <v>12.5</v>
       </c>
       <c r="G28"/>
-      <c r="H28" s="28"/>
+      <c r="H28" s="27"/>
       <c r="I28" s="11"/>
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
-    </row>
-    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L28" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="M28" s="29">
+        <v>12</v>
+      </c>
+      <c r="N28" s="29">
+        <v>12</v>
+      </c>
+      <c r="P28" s="60">
+        <v>42716</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="28">
+      <c r="D29" s="27">
         <v>42717</v>
       </c>
       <c r="E29" s="15">
         <v>15</v>
       </c>
-      <c r="F29" s="29">
+      <c r="F29" s="28">
         <f>(10*22+15*4)/(26)</f>
         <v>10.76923076923077</v>
       </c>
       <c r="G29"/>
-      <c r="H29" s="28"/>
+      <c r="H29" s="27"/>
       <c r="I29" s="11"/>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
-    </row>
-    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L29" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="M29" s="29">
+        <v>12</v>
+      </c>
+      <c r="N29" s="29">
+        <v>12</v>
+      </c>
+      <c r="P29" s="60">
+        <v>42720</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="28">
+      <c r="D30" s="27">
         <v>42721</v>
       </c>
       <c r="E30" s="15">
         <v>20</v>
       </c>
-      <c r="F30" s="29">
+      <c r="F30" s="28">
         <f>(10*36+20*6)/(36+6)</f>
         <v>11.428571428571429</v>
       </c>
-      <c r="H30" s="28"/>
+      <c r="H30" s="27"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-    </row>
-    <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L30" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="M30" s="29">
+        <v>12</v>
+      </c>
+      <c r="N30" s="29">
+        <v>12</v>
+      </c>
+      <c r="P30" s="60">
+        <v>42725</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F31" s="26">
         <f>(F30-F28)</f>
         <v>-1.0714285714285712</v>
       </c>
-      <c r="H31" s="25"/>
-      <c r="I31" s="26"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="25"/>
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-    </row>
-    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L31" s="53"/>
+      <c r="M31" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="N31" s="56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
         <v>32</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="H32" s="25"/>
+      <c r="H32" s="24"/>
       <c r="I32" s="11"/>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
     </row>
     <row r="33" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="28">
+      <c r="D33" s="27">
         <v>42711</v>
       </c>
       <c r="E33" s="15">
         <v>15</v>
       </c>
-      <c r="F33" s="29">
+      <c r="F33" s="28">
         <f>(15*15)/(15)</f>
         <v>15</v>
       </c>
       <c r="G33"/>
-      <c r="H33" s="28"/>
+      <c r="H33" s="27"/>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
-      <c r="Q33" s="11" t="s">
+      <c r="Q33" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D34" s="28">
+      <c r="D34" s="27">
         <v>42717</v>
       </c>
       <c r="E34" s="15">
         <v>15</v>
       </c>
-      <c r="F34" s="29">
+      <c r="F34" s="28">
         <f>(15*11+10*8)/(11+8)</f>
         <v>12.894736842105264</v>
       </c>
       <c r="G34"/>
-      <c r="H34" s="28"/>
+      <c r="H34" s="27"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
+      <c r="P34" s="60">
+        <v>42716</v>
+      </c>
     </row>
     <row r="35" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="28">
+      <c r="D35" s="27">
         <v>42721</v>
       </c>
       <c r="E35" s="15">
         <v>15</v>
       </c>
-      <c r="F35" s="29">
+      <c r="F35" s="28">
         <f>(15*12+10*24)/(36)</f>
         <v>11.666666666666666</v>
       </c>
       <c r="G35"/>
-      <c r="H35" s="28"/>
+      <c r="H35" s="27"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
+      <c r="P35" s="60">
+        <v>42720</v>
+      </c>
     </row>
     <row r="36" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="11"/>
-      <c r="E36" s="26" t="s">
+      <c r="E36" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="F36" s="27">
+      <c r="F36" s="26">
         <f>(F35-F33)</f>
         <v>-3.3333333333333339</v>
       </c>
-      <c r="H36" s="25"/>
-      <c r="I36" s="26"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="25"/>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
+      <c r="P36" s="60">
+        <v>42725</v>
+      </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -2633,10 +3083,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2645,13 +3095,13 @@
     <col min="2" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="51" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
       <c r="B2" s="15" t="s">
         <v>117</v>
       </c>
@@ -2659,393 +3109,888 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24"/>
       <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="15"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="48">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="47">
         <v>42711</v>
       </c>
-      <c r="B4" s="51">
+      <c r="B4" s="50">
         <v>60</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="45">
         <f>(60*15+70*45)/60</f>
         <v>67.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="44">
         <v>42717</v>
       </c>
-      <c r="B5" s="50">
+      <c r="B5" s="49">
         <v>70</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="42">
         <f>(70*45+80*6)/(45+6)</f>
         <v>71.17647058823529</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="44">
         <v>42721</v>
       </c>
       <c r="B6" s="49">
         <v>90</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="42">
         <f>(90*30+80*22)/(52)</f>
         <v>85.769230769230774</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="27">
-        <f>(C6-C4)</f>
-        <v>18.269230769230774</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="11" t="s">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="41">
+        <v>42727</v>
+      </c>
+      <c r="B7" s="48">
+        <v>100</v>
+      </c>
+      <c r="C7" s="39">
+        <f>(100*10+90*10+80*20)/(40)</f>
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="26">
+        <f>(C7-C4)</f>
+        <v>20</v>
+      </c>
+      <c r="D8" s="58">
+        <f>C8/B7</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="30"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="48">
+      <c r="C9" s="29"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="47">
         <v>42711</v>
       </c>
-      <c r="B9" s="51">
+      <c r="B10" s="50">
         <v>25</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C10" s="45">
         <f>(25*135+27.5*45)/(45*4)</f>
         <v>25.625</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="44">
         <v>42717</v>
       </c>
-      <c r="B10" s="50">
+      <c r="B11" s="49">
         <v>35</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C11" s="42">
         <f>(30*45+35*36+30*23+25*45)/(45+36+23+45)</f>
         <v>29.697986577181208</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="44">
         <v>42721</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B12" s="49">
         <v>35</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C12" s="42">
         <f>(35*45+30*45+30*29)/(45+45+29)</f>
         <v>31.890756302521009</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="27">
-        <f>(C11-C9)</f>
-        <v>6.2657563025210088</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="11" t="s">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="41">
+        <v>42727</v>
+      </c>
+      <c r="B13" s="48">
+        <v>50</v>
+      </c>
+      <c r="C13" s="39">
+        <f>(50*20+35*36+30*45+30*29)/(20+36+45+29)</f>
+        <v>34.46153846153846</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="26">
+        <f>(C13-C10)</f>
+        <v>8.8365384615384599</v>
+      </c>
+      <c r="D14" s="58">
+        <f>C14/B13</f>
+        <v>0.17673076923076919</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="27"/>
+      <c r="B15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="30"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="48">
+      <c r="C15" s="29"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="47">
         <v>42711</v>
       </c>
-      <c r="B14" s="51">
+      <c r="B16" s="50">
         <v>70</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C16" s="45">
         <f>(70*24+60*24)/(48)</f>
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="44">
         <v>42717</v>
       </c>
-      <c r="B15" s="50">
+      <c r="B17" s="49">
         <v>80</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C17" s="42">
         <f>(80*15+70*39)/(15+39)</f>
         <v>72.777777777777771</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="42">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="44">
         <v>42721</v>
       </c>
-      <c r="B16" s="49">
+      <c r="B18" s="49">
         <v>90</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C18" s="42">
         <f>(90*24+80*24)/(48)</f>
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="27">
-        <f>(C16-C14)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
-      <c r="B18" s="11" t="s">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="41">
+        <v>42727</v>
+      </c>
+      <c r="B19" s="48">
+        <v>90</v>
+      </c>
+      <c r="C19" s="39">
+        <f>(90*31+80*12)/(31+12)</f>
+        <v>87.20930232558139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" s="26">
+        <f>(C19-C16)</f>
+        <v>22.20930232558139</v>
+      </c>
+      <c r="D20" s="58">
+        <f>C20/B19</f>
+        <v>0.24677002583979324</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27"/>
+      <c r="B21" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="30"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="48">
+      <c r="C21" s="29"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="47">
         <v>42711</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B22" s="46">
         <v>30</v>
       </c>
-      <c r="C19" s="46">
+      <c r="C22" s="45">
         <f>(30*30+40*2)/(32)</f>
         <v>30.625</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="44">
         <v>42717</v>
       </c>
-      <c r="B20" s="50">
+      <c r="B23" s="49">
         <v>30</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C23" s="42">
         <f>(30*32+20*15)/(32+15)</f>
         <v>26.808510638297872</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="42">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="44">
         <v>42721</v>
       </c>
-      <c r="B21" s="49">
+      <c r="B24" s="49">
         <v>40</v>
       </c>
-      <c r="C21" s="40">
+      <c r="C24" s="42">
         <f>(40*4+30*30)/(34)</f>
         <v>31.176470588235293</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="26" t="s">
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="41">
+        <v>42727</v>
+      </c>
+      <c r="B25" s="48">
+        <v>40</v>
+      </c>
+      <c r="C25" s="39">
+        <f>(40*8+30*23)/(8+23)</f>
+        <v>32.58064516129032</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="27"/>
+      <c r="B26" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="27">
-        <f>(C21-C19)</f>
+      <c r="C26" s="26">
+        <f>(C24-C22)</f>
         <v>0.55147058823529349</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
-      <c r="B23" s="11" t="s">
+      <c r="D26" s="58">
+        <f>C26/B25</f>
+        <v>1.3786764705882337E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27"/>
+      <c r="B27" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="30"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="48">
+      <c r="C27" s="29"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="47">
         <v>42711</v>
       </c>
-      <c r="B24" s="51">
+      <c r="B28" s="50">
         <v>15</v>
       </c>
-      <c r="C24" s="46">
+      <c r="C28" s="45">
         <f>(15*17)/(17)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="44">
         <v>42717</v>
       </c>
-      <c r="B25" s="50">
+      <c r="B29" s="49">
         <v>20</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C29" s="42">
         <f>(20*9+15*23)/(9+23)</f>
         <v>16.40625</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="42">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="44">
         <v>42721</v>
       </c>
-      <c r="B26" s="49">
+      <c r="B30" s="49">
         <v>20</v>
       </c>
-      <c r="C26" s="40">
+      <c r="C30" s="42">
         <f>(20*15+15*9)/(15+9)</f>
         <v>18.125</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
-      <c r="B27" s="26" t="s">
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="41">
+        <v>42727</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="27">
-        <f>(C26-C24)</f>
+      <c r="C32" s="26">
+        <f>(C30-C28)</f>
         <v>3.125</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
-      <c r="B28" s="11" t="s">
+      <c r="D32" s="58">
+        <f>C32/B30</f>
+        <v>0.15625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="27"/>
+      <c r="B33" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="30"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="48">
+      <c r="C33" s="29"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="47">
         <v>42711</v>
       </c>
-      <c r="B29" s="47">
+      <c r="B34" s="46">
         <v>15</v>
       </c>
-      <c r="C29" s="46">
+      <c r="C34" s="45">
         <f>(10*12+15*12)/(24)</f>
         <v>12.5</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D34" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="44">
         <v>42717</v>
       </c>
-      <c r="B30" s="44">
+      <c r="B35" s="43">
         <v>15</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C35" s="42">
         <f>(10*22+15*4)/(26)</f>
         <v>10.76923076923077</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="42">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="44">
         <v>42721</v>
       </c>
-      <c r="B31" s="41">
+      <c r="B36" s="43">
         <v>20</v>
       </c>
-      <c r="C31" s="40">
+      <c r="C36" s="42">
         <f>(10*36+20*6)/(36+6)</f>
         <v>11.428571428571429</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="26" t="s">
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="41">
+        <v>42727</v>
+      </c>
+      <c r="B37" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="27">
-        <f>(C31-C29)</f>
+      <c r="C38" s="26">
+        <f>(C36-C34)</f>
         <v>-1.0714285714285712</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="25"/>
-      <c r="B33" s="11" t="s">
+      <c r="D38" s="58">
+        <f>C38/B36</f>
+        <v>-5.3571428571428562E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="24"/>
+      <c r="B39" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="15"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="48">
+      <c r="C39" s="15"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="47">
         <v>42711</v>
       </c>
-      <c r="B34" s="47">
+      <c r="B40" s="46">
         <v>15</v>
       </c>
-      <c r="C34" s="46">
+      <c r="C40" s="45">
         <f>(15*15)/(15)</f>
         <v>15</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D40" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="44">
         <v>42717</v>
       </c>
-      <c r="B35" s="44">
+      <c r="B41" s="43">
         <v>15</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C41" s="42">
         <f>(15*11+10*8)/(11+8)</f>
         <v>12.894736842105264</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="42">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="44">
         <v>42721</v>
       </c>
-      <c r="B36" s="41">
+      <c r="B42" s="43">
         <v>15</v>
       </c>
-      <c r="C36" s="40">
+      <c r="C42" s="42">
         <f>(15*12+10*24)/(36)</f>
         <v>11.666666666666666</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="26" t="s">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="41">
+        <v>42727</v>
+      </c>
+      <c r="B43" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="24"/>
+      <c r="B44" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C37" s="27">
-        <f>(C36-C34)</f>
+      <c r="C44" s="26">
+        <f>(C42-C40)</f>
         <v>-3.3333333333333339</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="C38" s="15"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="C39" s="15"/>
+      <c r="D44" s="58">
+        <f>C44/B42</f>
+        <v>-0.22222222222222227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="24"/>
+      <c r="C45" s="15"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="24"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="57" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="52"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="17"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24"/>
+      <c r="B3" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="47">
+        <v>42711</v>
+      </c>
+      <c r="B4" s="50">
+        <v>40</v>
+      </c>
+      <c r="C4" s="45">
+        <v>35</v>
+      </c>
+      <c r="G4" s="53"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="44">
+        <v>42717</v>
+      </c>
+      <c r="B5" s="49">
+        <v>40</v>
+      </c>
+      <c r="C5" s="42">
+        <v>36.25</v>
+      </c>
+      <c r="G5" s="53"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="54"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="44">
+        <v>42721</v>
+      </c>
+      <c r="B6" s="49">
+        <v>50</v>
+      </c>
+      <c r="C6" s="42">
+        <v>40.625</v>
+      </c>
+      <c r="G6" s="53"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="54"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="26">
+        <f>(C6-C4)</f>
+        <v>5.625</v>
+      </c>
+      <c r="D7" s="58">
+        <f>C7/B6</f>
+        <v>0.1125</v>
+      </c>
+      <c r="G7" s="53"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="26"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
+      <c r="B8" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="47">
+        <v>42711</v>
+      </c>
+      <c r="B9" s="50">
+        <v>25</v>
+      </c>
+      <c r="C9" s="45">
+        <v>23.333333333333332</v>
+      </c>
+      <c r="G9" s="53"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="54"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="44">
+        <v>42717</v>
+      </c>
+      <c r="B10" s="49">
+        <v>30</v>
+      </c>
+      <c r="C10" s="42">
+        <v>26.25</v>
+      </c>
+      <c r="G10" s="53"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="54"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="44">
+        <v>42721</v>
+      </c>
+      <c r="B11" s="49">
+        <v>30</v>
+      </c>
+      <c r="C11" s="42">
+        <v>30</v>
+      </c>
+      <c r="G11" s="53"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="26">
+        <f>(C11-C9)</f>
+        <v>6.6666666666666679</v>
+      </c>
+      <c r="D12" s="58">
+        <f>C12/B11</f>
+        <v>0.22222222222222227</v>
+      </c>
+      <c r="G12" s="53"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="26"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="27"/>
+      <c r="B13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="47">
+        <v>42711</v>
+      </c>
+      <c r="B14" s="50">
+        <v>65</v>
+      </c>
+      <c r="C14" s="45">
+        <v>51.666666666666664</v>
+      </c>
+      <c r="G14" s="53"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="54"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="44">
+        <v>42717</v>
+      </c>
+      <c r="B15" s="49">
+        <v>60</v>
+      </c>
+      <c r="C15" s="42">
+        <v>54.545454545454547</v>
+      </c>
+      <c r="G15" s="53"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="54"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="44">
+        <v>42721</v>
+      </c>
+      <c r="B16" s="49">
+        <v>70</v>
+      </c>
+      <c r="C16" s="42">
+        <v>61.836734693877553</v>
+      </c>
+      <c r="G16" s="53"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="54"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="26">
+        <f>(C16-C14)</f>
+        <v>10.170068027210888</v>
+      </c>
+      <c r="D17" s="58">
+        <f>C17/B16</f>
+        <v>0.14528668610301268</v>
+      </c>
+      <c r="G17" s="53"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="26"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27"/>
+      <c r="B18" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="47">
+        <v>42711</v>
+      </c>
+      <c r="B19" s="46">
+        <v>35</v>
+      </c>
+      <c r="C19" s="45">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="G19" s="53"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="55"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="44">
+        <v>42717</v>
+      </c>
+      <c r="B20" s="49">
+        <v>35</v>
+      </c>
+      <c r="C20" s="42">
+        <v>33.07692307692308</v>
+      </c>
+      <c r="G20" s="53"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="54"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="44">
+        <v>42721</v>
+      </c>
+      <c r="B21" s="49">
+        <v>40</v>
+      </c>
+      <c r="C21" s="42">
+        <v>36</v>
+      </c>
+      <c r="G21" s="53"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="54"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="26">
+        <f>(C21-C19)</f>
+        <v>2.6666666666666643</v>
+      </c>
+      <c r="D22" s="58">
+        <f>C22/B21</f>
+        <v>6.666666666666661E-2</v>
+      </c>
+      <c r="G22" s="53"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="26"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="C23" s="15"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="G24" s="53"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G25" s="53"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G26" s="53"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G27" s="53"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="56"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G28" s="53"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G29" s="53"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G30" s="53"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G31" s="53"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G32" s="53"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="56"/>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="52"/>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="52"/>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="52"/>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="52"/>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="52"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
(+)    added new workout plan, and added contents for juicing in diet
</commit_message>
<xml_diff>
--- a/Suppl/Plan 1.0 - lifting.xlsx
+++ b/Suppl/Plan 1.0 - lifting.xlsx
@@ -9,17 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Dec Plan '16 - r0" sheetId="2" r:id="rId1"/>
     <sheet name="Dec '16 Log" sheetId="3" r:id="rId2"/>
     <sheet name="BB Check" sheetId="4" r:id="rId3"/>
     <sheet name="Legs Check" sheetId="5" r:id="rId4"/>
+    <sheet name="ShTr Check" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'BB Check'!$A$1:$D$45</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Legs Check'!$A$1:$D$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'ShTr Check'!$A$1:$D$38</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="130">
   <si>
     <t>Day 1</t>
   </si>
@@ -415,6 +417,12 @@
   </si>
   <si>
     <t>(12/26/16)</t>
+  </si>
+  <si>
+    <t>(12/29/16)</t>
+  </si>
+  <si>
+    <t>Machine Shoulder Press</t>
   </si>
 </sst>
 </file>
@@ -797,10 +805,10 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1153,10 +1161,10 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="59">
+      <c r="B2" s="60">
         <v>42711</v>
       </c>
-      <c r="C2" s="59"/>
+      <c r="C2" s="60"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -1915,7 +1923,7 @@
         <f>(40*12+30*12+35*12)/(12+12+12)</f>
         <v>35</v>
       </c>
-      <c r="P3" s="60">
+      <c r="P3" s="59">
         <v>42716</v>
       </c>
       <c r="Q3" s="29">
@@ -1962,7 +1970,7 @@
         <f>(40*12+35*36)/(48)</f>
         <v>36.25</v>
       </c>
-      <c r="P4" s="60">
+      <c r="P4" s="59">
         <v>42720</v>
       </c>
       <c r="Q4" s="29">
@@ -2009,7 +2017,7 @@
         <f>(50*8+40*12+35*12)/(8+12+12)</f>
         <v>40.625</v>
       </c>
-      <c r="P5" s="60">
+      <c r="P5" s="59">
         <v>42725</v>
       </c>
       <c r="Q5" s="29">
@@ -2120,7 +2128,7 @@
         <f>(20*10+25*20)/(30)</f>
         <v>23.333333333333332</v>
       </c>
-      <c r="P8" s="60">
+      <c r="P8" s="59">
         <v>42716</v>
       </c>
       <c r="Q8" s="29">
@@ -2166,7 +2174,7 @@
         <f>(25*30+30*10)/(40)</f>
         <v>26.25</v>
       </c>
-      <c r="P9" s="60">
+      <c r="P9" s="59">
         <v>42720</v>
       </c>
       <c r="Q9" s="29">
@@ -2208,7 +2216,7 @@
         <f>(30*38)/(38)</f>
         <v>30</v>
       </c>
-      <c r="P10" s="60">
+      <c r="P10" s="59">
         <v>42725</v>
       </c>
       <c r="Q10" s="29">
@@ -2317,7 +2325,7 @@
         <f>(50*30+60*6)/(36)</f>
         <v>51.666666666666664</v>
       </c>
-      <c r="P13" s="60">
+      <c r="P13" s="59">
         <v>42716</v>
       </c>
       <c r="Q13" s="29">
@@ -2364,7 +2372,7 @@
         <f>(50*15+55*30+60*10)/(15+30+10)</f>
         <v>54.545454545454547</v>
       </c>
-      <c r="P14" s="60">
+      <c r="P14" s="59">
         <v>42720</v>
       </c>
       <c r="Q14" s="29">
@@ -2411,7 +2419,7 @@
         <f>(70*9+60*40)/(49)</f>
         <v>61.836734693877553</v>
       </c>
-      <c r="P15" s="60">
+      <c r="P15" s="59">
         <v>42725</v>
       </c>
       <c r="Q15" s="29">
@@ -2519,7 +2527,7 @@
         <f>(30*8+35*16)/(24)</f>
         <v>33.333333333333336</v>
       </c>
-      <c r="P18" s="60">
+      <c r="P18" s="59">
         <v>42716</v>
       </c>
       <c r="Q18" s="29">
@@ -2566,7 +2574,7 @@
         <f>(30*15+35*24)/(39)</f>
         <v>33.07692307692308</v>
       </c>
-      <c r="P19" s="60">
+      <c r="P19" s="59">
         <v>42720</v>
       </c>
       <c r="Q19" s="29">
@@ -2613,7 +2621,7 @@
         <f>(35*24+40*6)/(30)</f>
         <v>36</v>
       </c>
-      <c r="P20" s="60">
+      <c r="P20" s="59">
         <v>42725</v>
       </c>
       <c r="Q20" s="29">
@@ -2722,7 +2730,7 @@
       <c r="N23" s="29">
         <v>16</v>
       </c>
-      <c r="P23" s="60">
+      <c r="P23" s="59">
         <v>42716</v>
       </c>
       <c r="Q23" s="29"/>
@@ -2762,7 +2770,7 @@
       <c r="N24" s="29">
         <v>16</v>
       </c>
-      <c r="P24" s="60">
+      <c r="P24" s="59">
         <v>42720</v>
       </c>
       <c r="Q24" s="29"/>
@@ -2799,7 +2807,7 @@
       <c r="N25" s="29">
         <v>16</v>
       </c>
-      <c r="P25" s="60">
+      <c r="P25" s="59">
         <v>42725</v>
       </c>
       <c r="Q25" s="29"/>
@@ -2880,7 +2888,7 @@
       <c r="N28" s="29">
         <v>12</v>
       </c>
-      <c r="P28" s="60">
+      <c r="P28" s="59">
         <v>42716</v>
       </c>
     </row>
@@ -2912,7 +2920,7 @@
       <c r="N29" s="29">
         <v>12</v>
       </c>
-      <c r="P29" s="60">
+      <c r="P29" s="59">
         <v>42720</v>
       </c>
     </row>
@@ -2943,7 +2951,7 @@
       <c r="N30" s="29">
         <v>12</v>
       </c>
-      <c r="P30" s="60">
+      <c r="P30" s="59">
         <v>42725</v>
       </c>
     </row>
@@ -3021,7 +3029,7 @@
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
-      <c r="P34" s="60">
+      <c r="P34" s="59">
         <v>42716</v>
       </c>
     </row>
@@ -3041,7 +3049,7 @@
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
-      <c r="P35" s="60">
+      <c r="P35" s="59">
         <v>42720</v>
       </c>
     </row>
@@ -3058,7 +3066,7 @@
       <c r="I36" s="25"/>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
-      <c r="P36" s="60">
+      <c r="P36" s="59">
         <v>42725</v>
       </c>
     </row>
@@ -3616,8 +3624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,4 +4001,446 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24"/>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="15"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="47">
+        <v>42716</v>
+      </c>
+      <c r="B4" s="50">
+        <v>10</v>
+      </c>
+      <c r="C4" s="45">
+        <f>(10*27+5*10)/(37)</f>
+        <v>8.6486486486486491</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="44">
+        <v>42720</v>
+      </c>
+      <c r="B5" s="49">
+        <v>15</v>
+      </c>
+      <c r="C5" s="42">
+        <f>(15*10+10*10+5*10)/(30)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="41">
+        <v>42725</v>
+      </c>
+      <c r="B6" s="48">
+        <v>15</v>
+      </c>
+      <c r="C6" s="39">
+        <f>(15*19+10*10)/(29)</f>
+        <v>13.275862068965518</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="26">
+        <f>C6-C4</f>
+        <v>4.6272134203168687</v>
+      </c>
+      <c r="D7" s="58">
+        <f>C7/B6</f>
+        <v>0.30848089468779122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="29"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="47">
+        <v>42716</v>
+      </c>
+      <c r="B9" s="50">
+        <v>5</v>
+      </c>
+      <c r="C9" s="45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="44">
+        <v>42720</v>
+      </c>
+      <c r="B10" s="49">
+        <v>10</v>
+      </c>
+      <c r="C10" s="42">
+        <f>(5*40+10*20)/(60)</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="41">
+        <v>42725</v>
+      </c>
+      <c r="B11" s="48">
+        <v>10</v>
+      </c>
+      <c r="C11" s="39">
+        <f>(10*21+5*40)/(61)</f>
+        <v>6.721311475409836</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="26">
+        <f>C11-C9</f>
+        <v>1.721311475409836</v>
+      </c>
+      <c r="D12" s="58">
+        <f>C12/B11</f>
+        <v>0.1721311475409836</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="27"/>
+      <c r="B13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="29"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="47">
+        <v>42716</v>
+      </c>
+      <c r="B14" s="50">
+        <v>50</v>
+      </c>
+      <c r="C14" s="45">
+        <f>(40*30+50*5)/(35)</f>
+        <v>41.428571428571431</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="44">
+        <v>42720</v>
+      </c>
+      <c r="B15" s="49">
+        <v>50</v>
+      </c>
+      <c r="C15" s="42">
+        <f>(50*18+45*7+40*10)/(18+7+10)</f>
+        <v>46.142857142857146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="41">
+        <v>42725</v>
+      </c>
+      <c r="B16" s="48">
+        <v>60</v>
+      </c>
+      <c r="C16" s="39">
+        <f>(60*10+55*16+50*10)/(10+16+10)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="26">
+        <f>C16-C14</f>
+        <v>13.571428571428569</v>
+      </c>
+      <c r="D17" s="58">
+        <f>C17/B16</f>
+        <v>0.22619047619047616</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27"/>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="29"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="47">
+        <v>42716</v>
+      </c>
+      <c r="B19" s="46">
+        <v>60</v>
+      </c>
+      <c r="C19" s="45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="44">
+        <v>42720</v>
+      </c>
+      <c r="B20" s="49">
+        <v>80</v>
+      </c>
+      <c r="C20" s="42">
+        <f>(60*30+70*15+80*15)/(60)</f>
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="41">
+        <v>42725</v>
+      </c>
+      <c r="B21" s="48">
+        <v>80</v>
+      </c>
+      <c r="C21" s="39">
+        <f>(80*23+60*15)/(23+15)</f>
+        <v>72.10526315789474</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="26">
+        <f>C21-C19</f>
+        <v>12.10526315789474</v>
+      </c>
+      <c r="D22" s="58">
+        <f>C22/B21</f>
+        <v>0.15131578947368424</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27"/>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="29"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="47">
+        <v>42716</v>
+      </c>
+      <c r="B24" s="50">
+        <v>60</v>
+      </c>
+      <c r="C24" s="45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="44">
+        <v>42720</v>
+      </c>
+      <c r="B25" s="49">
+        <v>70</v>
+      </c>
+      <c r="C25" s="42">
+        <f>(70*21+60*20)/(41)</f>
+        <v>65.121951219512198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="41">
+        <v>42725</v>
+      </c>
+      <c r="B26" s="48">
+        <v>70</v>
+      </c>
+      <c r="C26" s="39">
+        <f>(70*20+50*2)/(22)</f>
+        <v>68.181818181818187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="26">
+        <f>(C26-C24)</f>
+        <v>8.181818181818187</v>
+      </c>
+      <c r="D27" s="58">
+        <f>C27/B26</f>
+        <v>0.11688311688311696</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="27"/>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="29"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="47">
+        <v>42716</v>
+      </c>
+      <c r="B29" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="44">
+        <v>42720</v>
+      </c>
+      <c r="B30" s="43">
+        <v>8</v>
+      </c>
+      <c r="C30" s="42">
+        <f>AVERAGE(8,7,4,2)</f>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="41">
+        <v>42725</v>
+      </c>
+      <c r="B31" s="40">
+        <v>10</v>
+      </c>
+      <c r="C31" s="39">
+        <f>AVERAGE(10,6,6)</f>
+        <v>7.333333333333333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="26">
+        <v>0</v>
+      </c>
+      <c r="D32" s="58">
+        <f>C32/B31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="24"/>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="15"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="47">
+        <v>42716</v>
+      </c>
+      <c r="B34" s="46">
+        <v>25</v>
+      </c>
+      <c r="C34" s="45">
+        <f>(20*30+25*15)/(45)</f>
+        <v>21.666666666666668</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="44">
+        <v>42720</v>
+      </c>
+      <c r="B35" s="43">
+        <v>30</v>
+      </c>
+      <c r="C35" s="42">
+        <f>(25*45+30*15)/(60)</f>
+        <v>26.25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="41">
+        <v>42725</v>
+      </c>
+      <c r="B36" s="40">
+        <v>30</v>
+      </c>
+      <c r="C36" s="39">
+        <f>(30*30+25*15)/(45)</f>
+        <v>28.333333333333332</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
+      <c r="B37" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="26">
+        <f>(C36-C34)</f>
+        <v>6.6666666666666643</v>
+      </c>
+      <c r="D37" s="58">
+        <f>C37/B36</f>
+        <v>0.22222222222222215</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="C38" s="15"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="57" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D7 D12 D17 D22 D27 D32 D37" evalError="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>